<commit_message>
Refactor driver factories and enhance Jenkins compatibility
Updated driver factories to enable headless mode for Jenkins executions. Modified properties and listeners to manage executionType and prevent report display for Jenkins. Updated Jenkinsfile and test data to align with Jenkins execution needs.
</commit_message>
<xml_diff>
--- a/src/test/resources/homePageTestData.xlsx
+++ b/src/test/resources/homePageTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\IdeaProjects\demoblaze\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD2B9BF-4002-45AE-A3B1-0957529387D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3233624E-AC9C-400D-851D-3E40421A5691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E09886AD-8734-4170-BB23-AF7D27A0C7B0}"/>
+    <workbookView xWindow="2832" yWindow="2136" windowWidth="17280" windowHeight="8880" xr2:uid="{E09886AD-8734-4170-BB23-AF7D27A0C7B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>firstPageElementsCount</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Actual</t>
-  </si>
-  <si>
-    <t>20</t>
   </si>
 </sst>
 </file>
@@ -451,7 +448,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>